<commit_message>
Updates to files accounting for tax revenue correctly, adjusting to only be deficit spending, and fixing an error in DLIM
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/ctrl-settings/gra/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\ctrl-settings\GRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE535FE-2280-DF4E-AC32-9EA66AB8F26C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5096C2B-4EE5-4923-A73D-13A8F2B73320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="2680" windowWidth="25660" windowHeight="13520" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="698" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -710,14 +710,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="80.83203125" customWidth="1"/>
+    <col min="2" max="2" width="80.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +725,7 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -733,72 +733,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -806,7 +806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -814,7 +814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -822,7 +822,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -830,7 +830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -838,114 +838,114 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="13"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -965,12 +965,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -978,16 +978,16 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B15:F15)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -995,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1033,12 +1033,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1046,16 +1046,16 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B16:F16)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1099,37 +1099,37 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1299,12 +1299,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C15" s="14">
         <v>0</v>
@@ -1319,12 +1319,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -1339,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>52</v>
       </c>
@@ -1349,12 +1349,12 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1549,13 +1549,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="10">
         <f t="shared" ref="B29:F29" si="7">IFERROR(B15/SUM($B15:$F15),1/COUNT($B15:$F15))</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C29" s="10">
         <f t="shared" si="7"/>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="D29" s="10">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E29" s="10">
         <f t="shared" si="7"/>
@@ -1574,21 +1574,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="10">
         <f t="shared" ref="B30:F30" si="8">IFERROR(B16/SUM($B16:$F16),1/COUNT($B16:$F16))</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="C30" s="10">
         <f t="shared" si="8"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="D30" s="10">
         <f t="shared" si="8"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="E30" s="10">
         <f t="shared" si="8"/>
@@ -1617,12 +1617,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1685,12 +1685,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1753,12 +1753,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1821,12 +1821,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1889,12 +1889,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1957,12 +1957,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2025,12 +2025,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>

</xml_diff>